<commit_message>
Update boutprocess and size class key
</commit_message>
<xml_diff>
--- a/helperfiles/Sizeclass_key.xlsx
+++ b/helperfiles/Sizeclass_key.xlsx
@@ -1,20 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Tinker\OneDrive\Documents\Nhydra\Projects\SOFA2\SOFA\data\WASH_2010_2020_SA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/SOFA2/SOFA/helperfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE3F950-568B-4C36-9F77-1DE89E9B9BC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{441CB33B-7DFA-428E-8B93-66C504E3CC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27930" windowHeight="15165" xr2:uid="{58EDC278-7532-4510-8B21-A021042D543C}"/>
+    <workbookView xWindow="180" yWindow="645" windowWidth="28635" windowHeight="13680" xr2:uid="{58EDC278-7532-4510-8B21-A021042D543C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$2</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$E$2</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">13</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -130,6 +159,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,6 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,15 +540,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0895321-839B-42DE-A004-41E02DA7DC65}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -529,13 +565,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <f>(C2-1)+1/6</f>
-        <v>0.16666666666666666</v>
+        <v>0.26</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -543,8 +578,9 @@
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -557,8 +593,9 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -569,8 +606,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -584,8 +623,9 @@
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -599,13 +639,14 @@
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -613,20 +654,23 @@
       <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2</v>
       </c>
       <c r="B8" s="2">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="3"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -640,8 +684,9 @@
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -655,13 +700,14 @@
       <c r="D10" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="C11" s="2">
         <v>3</v>
@@ -669,20 +715,23 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
       <c r="B12" s="2">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="C12" s="2">
         <v>3</v>
       </c>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="3"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -696,8 +745,9 @@
       <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -711,13 +761,14 @@
       <c r="D14" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>0.5</v>
+        <v>3.5</v>
       </c>
       <c r="C15" s="2">
         <v>4</v>
@@ -725,20 +776,23 @@
       <c r="D15" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>4</v>
       </c>
       <c r="B16" s="2">
-        <v>0.5</v>
+        <v>3.5</v>
       </c>
       <c r="C16" s="2">
         <v>4</v>
       </c>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -752,13 +806,14 @@
       <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="2">
-        <v>4</v>
+        <v>4.1666670000000003</v>
       </c>
       <c r="C18" s="2">
         <v>4</v>
@@ -766,6 +821,7 @@
       <c r="D18" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="E18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>